<commit_message>
remove make from script
</commit_message>
<xml_diff>
--- a/window_test/BigWindowTest.xlsx
+++ b/window_test/BigWindowTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\basill\research\steps\window_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE43901-2816-4A01-9730-D5DDA29CE0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E858F2A-72E0-45C8-A28A-B809A5075517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{84E3301A-F825-4024-A261-013B8CF6529A}"/>
   </bookViews>
@@ -3558,7 +3558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C63892F-D4CA-4456-8DA4-86BE7C49628E}">
   <dimension ref="A1:AM64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>

</xml_diff>